<commit_message>
We create some examples to better understand the database structure
</commit_message>
<xml_diff>
--- a/BD-Onboard.xlsx
+++ b/BD-Onboard.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alunosipca-my.sharepoint.com/personal/a20629_alunos_ipca_pt/Documents/IPCA/DWM/02_S1-DCS/TP/WIP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JR\Documents\Edu\Univ\DWM-IPCA\02_S1-DCS\TP\WIP\OnboardDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="187" documentId="11_9248381DC2F30A436F107A39913E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F99DEAA-B6AE-466D-AB20-C0411FE2B5CF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156E68BC-C2D9-4A55-B801-8E683DA679AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5760" yWindow="1752" windowWidth="17280" windowHeight="9024" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BD-Onboard" sheetId="1" r:id="rId1"/>
-    <sheet name="Folha1" sheetId="2" r:id="rId2"/>
+    <sheet name="BD-Onboard (testes)" sheetId="3" r:id="rId2"/>
+    <sheet name="Folha1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
   <si>
     <t>Base de Dados</t>
   </si>
@@ -209,13 +210,138 @@
   </si>
   <si>
     <t>vamos decidir depois</t>
+  </si>
+  <si>
+    <t>company name</t>
+  </si>
+  <si>
+    <t>passowrd</t>
+  </si>
+  <si>
+    <t>comercial 1</t>
+  </si>
+  <si>
+    <t>comercial 3</t>
+  </si>
+  <si>
+    <t>comercial 4</t>
+  </si>
+  <si>
+    <t>comercial 5</t>
+  </si>
+  <si>
+    <t>comercial 6</t>
+  </si>
+  <si>
+    <t>comercial 7</t>
+  </si>
+  <si>
+    <t>comercial 8</t>
+  </si>
+  <si>
+    <t>comercial 9</t>
+  </si>
+  <si>
+    <t>comercial 10</t>
+  </si>
+  <si>
+    <t>comercial 2</t>
+  </si>
+  <si>
+    <t>empresa xpto</t>
+  </si>
+  <si>
+    <t>andre</t>
+  </si>
+  <si>
+    <t>antonio</t>
+  </si>
+  <si>
+    <t>artur</t>
+  </si>
+  <si>
+    <t>r2022</t>
+  </si>
+  <si>
+    <t>comercial1@onboard.com</t>
+  </si>
+  <si>
+    <t>comercial2@onboard.com</t>
+  </si>
+  <si>
+    <t>cxpto 1</t>
+  </si>
+  <si>
+    <t>cxpto 2</t>
+  </si>
+  <si>
+    <t>cxpto1@xpto.com</t>
+  </si>
+  <si>
+    <t>cxpto2@xpto.com</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>Accounts (administrator)</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>pagina 1: adms de empresas</t>
+  </si>
+  <si>
+    <t>Pagina 2: comerceiais de empresas</t>
+  </si>
+  <si>
+    <t>Registar Conta (ADM)</t>
+  </si>
+  <si>
+    <t>Users (funcionarios)</t>
+  </si>
+  <si>
+    <t>Menu criar utilizador (ADM)</t>
+  </si>
+  <si>
+    <t>PAG 1:menu inserir utilizadores</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PAG 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> transações e vamos ver as transações individuais do utilizador</t>
+    </r>
+  </si>
+  <si>
+    <t>ALIMENTACAO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,16 +357,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -507,11 +653,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -567,6 +725,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -579,11 +740,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -899,56 +1100,56 @@
   <dimension ref="B2:S16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="C4" sqref="C4:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.88671875" style="1"/>
-    <col min="10" max="10" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="8.88671875" style="1"/>
-    <col min="14" max="14" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.77734375" style="1" customWidth="1"/>
-    <col min="18" max="19" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.85546875" style="1"/>
+    <col min="10" max="10" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="8.85546875" style="1"/>
+    <col min="14" max="14" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.7109375" style="1" customWidth="1"/>
+    <col min="18" max="19" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="19" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
-      <c r="H4" s="19" t="s">
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
+      <c r="H4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="21"/>
-      <c r="N4" s="19" t="s">
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="22"/>
+      <c r="N4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="21"/>
-    </row>
-    <row r="5" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="22"/>
+    </row>
+    <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
@@ -995,7 +1196,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C6" s="4">
         <v>1</v>
       </c>
@@ -1034,7 +1235,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="7">
         <v>2</v>
       </c>
@@ -1073,14 +1274,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="19" t="s">
+    <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="21"/>
-    </row>
-    <row r="13" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="22"/>
+    </row>
+    <row r="13" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
@@ -1088,7 +1289,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C14" s="10">
         <v>1</v>
       </c>
@@ -1096,7 +1297,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C15" s="12">
         <v>2</v>
       </c>
@@ -1104,7 +1305,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="14">
         <v>3</v>
       </c>
@@ -1126,23 +1327,527 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21980860-3ED3-4236-B456-9214120E1B2A}">
+  <dimension ref="B2:S39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.28515625" style="27" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.7109375" style="1" customWidth="1"/>
+    <col min="18" max="19" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
+      <c r="H4" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="22"/>
+      <c r="N4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="22"/>
+    </row>
+    <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="4">
+        <v>123456</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="5">
+        <v>123456</v>
+      </c>
+      <c r="N6" s="4">
+        <v>1</v>
+      </c>
+      <c r="O6" s="4">
+        <v>1</v>
+      </c>
+      <c r="P6" s="6">
+        <v>44509</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>3</v>
+      </c>
+      <c r="R6" s="4">
+        <v>6</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C7" s="25">
+        <v>2</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="4">
+        <v>123456</v>
+      </c>
+      <c r="H7" s="25">
+        <v>2</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="25">
+        <v>1</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="5">
+        <v>123456</v>
+      </c>
+      <c r="N7" s="25">
+        <v>2</v>
+      </c>
+      <c r="O7" s="25">
+        <v>1</v>
+      </c>
+      <c r="P7" s="26">
+        <v>44501</v>
+      </c>
+      <c r="Q7" s="25">
+        <v>2</v>
+      </c>
+      <c r="R7" s="25">
+        <v>20</v>
+      </c>
+      <c r="S7" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C8" s="25">
+        <v>3</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="4">
+        <v>123456</v>
+      </c>
+      <c r="H8" s="25">
+        <v>3</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="25">
+        <v>2</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" s="5">
+        <v>123456</v>
+      </c>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="4"/>
+      <c r="H9" s="25">
+        <v>4</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="J9" s="25">
+        <v>2</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" s="5">
+        <v>123456</v>
+      </c>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+    </row>
+    <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="4"/>
+      <c r="H10" s="7">
+        <v>5</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="8"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+    </row>
+    <row r="17" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="L18" s="32"/>
+      <c r="M18" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="N18" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="J19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="1">
+        <v>2</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" s="10">
+        <v>1</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L21" s="1">
+        <v>3</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C22" s="12">
+        <v>2</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" s="1">
+        <v>4</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="14">
+        <v>3</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L23" s="1">
+        <v>5</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="L24" s="1">
+        <v>6</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="L25" s="1">
+        <v>7</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="L26" s="1">
+        <v>8</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="L27" s="1">
+        <v>9</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="L28" s="1">
+        <v>10</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M29" s="24"/>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M30" s="24"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M31" s="24"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M32" s="24"/>
+    </row>
+    <row r="33" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="M33" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="36"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="36"/>
+    </row>
+    <row r="34" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="J34" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="K34" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="M34" s="24"/>
+    </row>
+    <row r="35" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="K35" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="M35" s="24"/>
+      <c r="N35" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O35" s="6">
+        <v>44509</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q35" s="37">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="M36" s="24"/>
+    </row>
+    <row r="37" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="M37" s="24"/>
+    </row>
+    <row r="38" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="M38" s="24"/>
+    </row>
+    <row r="39" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="M39" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="M33:S33"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="N4:S4"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="K6" r:id="rId1" xr:uid="{8A8A762A-B7E7-471E-AA59-31CF2E500441}"/>
+    <hyperlink ref="K7" r:id="rId2" xr:uid="{83738695-7ABB-4B89-B0EA-022F19AE12A1}"/>
+    <hyperlink ref="K8" r:id="rId3" xr:uid="{8F57AA61-C263-4330-804C-7EC8070D3E98}"/>
+    <hyperlink ref="K9" r:id="rId4" xr:uid="{3B05CF7C-D890-44CD-A32E-D265B4DC0B91}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101C0A5E-53D3-4EE9-8425-C86F54FEF2B4}">
   <dimension ref="B1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="21.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>53</v>
       </c>
@@ -1156,7 +1861,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>26</v>
       </c>
@@ -1170,7 +1875,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
         <v>30</v>
       </c>
@@ -1184,7 +1889,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
         <v>33</v>
       </c>
@@ -1198,7 +1903,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
         <v>36</v>
       </c>
@@ -1212,7 +1917,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="16"/>
       <c r="C7" s="16" t="s">
         <v>50</v>
@@ -1223,11 +1928,11 @@
       <c r="E7" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>38</v>
       </c>
@@ -1241,7 +1946,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
         <v>40</v>
       </c>
@@ -1255,7 +1960,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
       <c r="C10" s="16" t="s">
         <v>31</v>
@@ -1267,7 +1972,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="16"/>
       <c r="C11" s="16" t="s">
         <v>31</v>
@@ -1279,7 +1984,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
         <v>44</v>
       </c>
@@ -1293,7 +1998,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
         <v>47</v>
       </c>
@@ -1305,7 +2010,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="16"/>
       <c r="C14" s="16" t="s">
         <v>34</v>
@@ -1315,7 +2020,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="16"/>
       <c r="C15" s="16" t="s">
         <v>50</v>
@@ -1325,7 +2030,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Updating the restfull url table
</commit_message>
<xml_diff>
--- a/BD-Onboard.xlsx
+++ b/BD-Onboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JR\Documents\Edu\Univ\DWM-IPCA\02_S1-DCS\TP\WIP\OnboardDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156E68BC-C2D9-4A55-B801-8E683DA679AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CBDC55-C907-461C-B100-536ABBA3BCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BD-Onboard" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="100">
   <si>
     <t>Base de Dados</t>
   </si>
@@ -113,9 +113,6 @@
     <t>photo</t>
   </si>
   <si>
-    <t>/Accounts/Users/; &lt;userData&gt;</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -125,39 +122,24 @@
     <t>createAccount</t>
   </si>
   <si>
-    <t>/Accounts/Users/; { profile_id }</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
     <t>getAccount</t>
   </si>
   <si>
-    <t>/Accounts/Users/ { profile_id } &lt;profileData&gt;</t>
-  </si>
-  <si>
     <t>PUT</t>
   </si>
   <si>
     <t>updateAccount</t>
   </si>
   <si>
-    <t>/.../Users/; &lt;userData&gt;</t>
-  </si>
-  <si>
     <t>createUser</t>
   </si>
   <si>
-    <t>/.../Users/; { profile }</t>
-  </si>
-  <si>
     <t>getUser</t>
   </si>
   <si>
-    <t>/.../Users/; { profile_id } &lt;profileData&gt;</t>
-  </si>
-  <si>
     <t>updateUser</t>
   </si>
   <si>
@@ -167,18 +149,12 @@
     <t>doLogOut</t>
   </si>
   <si>
-    <t xml:space="preserve">/.../Users/Summary/ </t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
     <t>getUserSummary</t>
   </si>
   <si>
-    <t>/.../Users/</t>
-  </si>
-  <si>
     <t>createExpense</t>
   </si>
   <si>
@@ -207,9 +183,6 @@
   </si>
   <si>
     <t>DeleteUser</t>
-  </si>
-  <si>
-    <t>vamos decidir depois</t>
   </si>
   <si>
     <t>company name</t>
@@ -332,6 +305,54 @@
   </si>
   <si>
     <t>ALIMENTACAO</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Category (Fkey)</t>
+  </si>
+  <si>
+    <t>/Companies/Accounts/; &lt;accountData&gt;</t>
+  </si>
+  <si>
+    <t>/Companies/Users/; &lt;userData&gt;</t>
+  </si>
+  <si>
+    <t>/Companies/Accounts/ { account_id }</t>
+  </si>
+  <si>
+    <t>/Companies/Accounts/; { account_id } &lt;accountData&gt;</t>
+  </si>
+  <si>
+    <t>/Companies/Users/; { user_id }</t>
+  </si>
+  <si>
+    <t>/Companies/Users/; { user_id } &lt;userData&gt;</t>
+  </si>
+  <si>
+    <t>/Companies/Summary; { acc_id}</t>
+  </si>
+  <si>
+    <t>/Companies/Expenses; &lt;expenseData&gt;</t>
+  </si>
+  <si>
+    <t>/Companies/Expenses/ { expense_id} &lt;expenseData&gt;</t>
+  </si>
+  <si>
+    <t>doSignup</t>
+  </si>
+  <si>
+    <t>/Signup/</t>
+  </si>
+  <si>
+    <t>/Login/Users/; &lt;userData&gt;</t>
+  </si>
+  <si>
+    <t>Companies/LogOut/; &lt;userData&gt;</t>
   </si>
 </sst>
 </file>
@@ -386,7 +407,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -642,15 +663,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -669,7 +681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -725,7 +737,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -743,45 +788,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -1119,35 +1141,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
-      <c r="H4" s="20" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
+      <c r="H4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="22"/>
-      <c r="N4" s="20" t="s">
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
+      <c r="N4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="22"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="33"/>
     </row>
     <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
@@ -1276,10 +1298,10 @@
     </row>
     <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="22"/>
+      <c r="D12" s="33"/>
     </row>
     <row r="13" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
@@ -1330,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21980860-3ED3-4236-B456-9214120E1B2A}">
   <dimension ref="B2:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,46 +1364,46 @@
     <col min="5" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.28515625" style="27" customWidth="1"/>
+    <col min="11" max="11" width="32.28515625" style="22" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" style="1" customWidth="1"/>
     <col min="17" max="17" width="22.7109375" style="1" customWidth="1"/>
     <col min="18" max="19" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
-      <c r="H4" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="22"/>
-      <c r="N4" s="20" t="s">
+      <c r="C4" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
+      <c r="H4" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
+      <c r="N4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="22"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="33"/>
     </row>
     <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
@@ -1405,7 +1427,7 @@
       <c r="J5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="23" t="s">
         <v>2</v>
       </c>
       <c r="L5" s="3" t="s">
@@ -1418,15 +1440,15 @@
         <v>23</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S5" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="S5" s="27" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1438,7 +1460,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F6" s="4">
         <v>123456</v>
@@ -1447,13 +1469,13 @@
         <v>1</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="J6" s="4">
         <v>1</v>
       </c>
-      <c r="K6" s="31" t="s">
-        <v>76</v>
+      <c r="K6" s="26" t="s">
+        <v>67</v>
       </c>
       <c r="L6" s="5">
         <v>123456</v>
@@ -1478,113 +1500,113 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C7" s="25">
+      <c r="C7" s="20">
         <v>2</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>73</v>
+      <c r="D7" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>64</v>
       </c>
       <c r="F7" s="4">
         <v>123456</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="20">
         <v>2</v>
       </c>
-      <c r="I7" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="J7" s="25">
+      <c r="I7" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="20">
         <v>1</v>
       </c>
-      <c r="K7" s="31" t="s">
-        <v>77</v>
+      <c r="K7" s="26" t="s">
+        <v>68</v>
       </c>
       <c r="L7" s="5">
         <v>123456</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="20">
         <v>2</v>
       </c>
-      <c r="O7" s="25">
+      <c r="O7" s="20">
         <v>1</v>
       </c>
-      <c r="P7" s="26">
+      <c r="P7" s="21">
         <v>44501</v>
       </c>
-      <c r="Q7" s="25">
+      <c r="Q7" s="20">
         <v>2</v>
       </c>
-      <c r="R7" s="25">
+      <c r="R7" s="20">
         <v>20</v>
       </c>
-      <c r="S7" s="25" t="s">
+      <c r="S7" s="20" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C8" s="25">
+      <c r="C8" s="20">
         <v>3</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>74</v>
+      <c r="D8" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>65</v>
       </c>
       <c r="F8" s="4">
         <v>123456</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="20">
         <v>3</v>
       </c>
-      <c r="I8" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" s="25">
+      <c r="I8" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="20">
         <v>2</v>
       </c>
-      <c r="K8" s="29" t="s">
-        <v>80</v>
+      <c r="K8" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="L8" s="5">
         <v>123456</v>
       </c>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="4"/>
-      <c r="H9" s="25">
+      <c r="H9" s="20">
         <v>4</v>
       </c>
-      <c r="I9" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="J9" s="25">
+      <c r="I9" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="20">
         <v>2</v>
       </c>
-      <c r="K9" s="29" t="s">
-        <v>81</v>
+      <c r="K9" s="24" t="s">
+        <v>72</v>
       </c>
       <c r="L9" s="5">
         <v>123456</v>
       </c>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
     </row>
     <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="7"/>
@@ -1596,7 +1618,7 @@
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="30"/>
+      <c r="K10" s="25"/>
       <c r="L10" s="8"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
@@ -1607,18 +1629,18 @@
     </row>
     <row r="17" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I18" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="L18" s="32"/>
-      <c r="M18" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="N18" s="28" t="s">
+      <c r="I18" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="L18" s="36"/>
+      <c r="M18" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="N18" s="23" t="s">
         <v>2</v>
       </c>
       <c r="O18" s="3" t="s">
@@ -1626,18 +1648,18 @@
       </c>
     </row>
     <row r="19" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="22"/>
+      <c r="D19" s="33"/>
       <c r="J19" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L19" s="1">
         <v>1</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1654,7 +1676,7 @@
         <v>2</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
@@ -1665,13 +1687,13 @@
         <v>16</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="L21" s="1">
         <v>3</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.25">
@@ -1685,7 +1707,7 @@
         <v>4</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1699,7 +1721,7 @@
         <v>5</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
@@ -1707,7 +1729,7 @@
         <v>6</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.25">
@@ -1715,7 +1737,7 @@
         <v>7</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.25">
@@ -1723,7 +1745,7 @@
         <v>8</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.25">
@@ -1731,7 +1753,7 @@
         <v>9</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.25">
@@ -1739,73 +1761,73 @@
         <v>10</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M29" s="24"/>
+      <c r="M29" s="19"/>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M30" s="24"/>
+      <c r="M30" s="19"/>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M31" s="24"/>
+        <v>78</v>
+      </c>
+      <c r="M31" s="19"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M32" s="24"/>
+      <c r="M32" s="19"/>
     </row>
     <row r="33" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M33" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="N33" s="36"/>
-      <c r="O33" s="36"/>
-      <c r="P33" s="36"/>
-      <c r="Q33" s="36"/>
-      <c r="R33" s="36"/>
-      <c r="S33" s="36"/>
+      <c r="M33" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="35"/>
     </row>
     <row r="34" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J34" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="K34" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="M34" s="24"/>
+      <c r="J34" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="K34" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="M34" s="19"/>
     </row>
     <row r="35" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="K35" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="M35" s="24"/>
+      <c r="K35" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="M35" s="19"/>
       <c r="N35" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="O35" s="6">
         <v>44509</v>
       </c>
       <c r="P35" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q35" s="37">
+        <v>83</v>
+      </c>
+      <c r="Q35" s="30">
         <v>200</v>
       </c>
     </row>
     <row r="36" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M36" s="24"/>
+      <c r="M36" s="19"/>
     </row>
     <row r="37" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M37" s="24"/>
+      <c r="M37" s="19"/>
     </row>
     <row r="38" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M38" s="24"/>
+      <c r="M38" s="19"/>
     </row>
     <row r="39" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M39" s="24"/>
+      <c r="M39" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1832,215 +1854,245 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101C0A5E-53D3-4EE9-8425-C86F54FEF2B4}">
-  <dimension ref="B1:F16"/>
+  <dimension ref="B1:G17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="55.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="5" t="s">
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="38" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="D4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="16" t="s">
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="17" t="s">
+      <c r="D5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="16" t="s">
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="17" t="s">
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="40"/>
+      <c r="G9" s="41"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="17" t="s">
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="16"/>
-      <c r="C10" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="16"/>
-      <c r="C11" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="7"/>
+      <c r="C17" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="16"/>
-      <c r="C15" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New version of our database with users, companies, roles, transaction tags and transactions
</commit_message>
<xml_diff>
--- a/BD-Onboard.xlsx
+++ b/BD-Onboard.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JR\Documents\Edu\Univ\DWM-IPCA\02_S1-DCS\TP\WIP\OnboardDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CBDC55-C907-461C-B100-536ABBA3BCAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D683FF-7960-4FF6-9546-E101B5ABC364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BD-Onboard" sheetId="1" r:id="rId1"/>
-    <sheet name="BD-Onboard (testes)" sheetId="3" r:id="rId2"/>
-    <sheet name="Folha1" sheetId="2" r:id="rId3"/>
+    <sheet name="BD-Onboard (testes) (2)" sheetId="4" r:id="rId2"/>
+    <sheet name="BD-Onboard v2" sheetId="3" r:id="rId3"/>
+    <sheet name="Folha1" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="109">
   <si>
     <t>Base de Dados</t>
   </si>
@@ -141,9 +142,6 @@
   </si>
   <si>
     <t>updateUser</t>
-  </si>
-  <si>
-    <t>doLogin</t>
   </si>
   <si>
     <t>doLogOut</t>
@@ -334,25 +332,55 @@
     <t>/Companies/Users/; { user_id } &lt;userData&gt;</t>
   </si>
   <si>
-    <t>/Companies/Summary; { acc_id}</t>
-  </si>
-  <si>
     <t>/Companies/Expenses; &lt;expenseData&gt;</t>
   </si>
   <si>
     <t>/Companies/Expenses/ { expense_id} &lt;expenseData&gt;</t>
   </si>
   <si>
-    <t>doSignup</t>
-  </si>
-  <si>
-    <t>/Signup/</t>
-  </si>
-  <si>
-    <t>/Login/Users/; &lt;userData&gt;</t>
-  </si>
-  <si>
     <t>Companies/LogOut/; &lt;userData&gt;</t>
+  </si>
+  <si>
+    <t>/Companies/Summary; { user_id}</t>
+  </si>
+  <si>
+    <t>doLoginUser</t>
+  </si>
+  <si>
+    <t>/Login/Accounts/; &lt;AccountData&gt;</t>
+  </si>
+  <si>
+    <t>/Login/Users/; &lt;UserData&gt;</t>
+  </si>
+  <si>
+    <t>doLoginAccount</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Companies</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>adm1</t>
+  </si>
+  <si>
+    <t>só precisa de 1 login com a logica toda</t>
+  </si>
+  <si>
+    <t>adm2</t>
+  </si>
+  <si>
+    <t>abc@onboard.com</t>
   </si>
 </sst>
 </file>
@@ -681,7 +709,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -773,6 +801,25 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -791,19 +838,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -1125,53 +1159,53 @@
       <selection activeCell="C4" sqref="C4:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.85546875" style="1"/>
-    <col min="10" max="10" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="8.85546875" style="1"/>
-    <col min="14" max="14" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.7109375" style="1" customWidth="1"/>
-    <col min="18" max="19" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.6640625" style="1" customWidth="1"/>
+    <col min="18" max="19" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-    </row>
-    <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="31" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+    </row>
+    <row r="3" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
-      <c r="H4" s="31" t="s">
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40"/>
+      <c r="H4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="33"/>
-      <c r="N4" s="31" t="s">
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="40"/>
+      <c r="N4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="33"/>
-    </row>
-    <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="40"/>
+    </row>
+    <row r="5" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1218,7 +1252,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C6" s="4">
         <v>1</v>
       </c>
@@ -1257,7 +1291,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="7">
         <v>2</v>
       </c>
@@ -1296,14 +1330,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="31" t="s">
+    <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="33"/>
-    </row>
-    <row r="13" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="40"/>
+    </row>
+    <row r="13" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
@@ -1311,7 +1345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C14" s="10">
         <v>1</v>
       </c>
@@ -1319,7 +1353,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C15" s="12">
         <v>2</v>
       </c>
@@ -1327,7 +1361,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="14">
         <v>3</v>
       </c>
@@ -1349,63 +1383,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21980860-3ED3-4236-B456-9214120E1B2A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1D65F-0224-440E-8E41-D38BFBBE509B}">
   <dimension ref="B2:S39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="9.140625" style="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="8.88671875" style="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.28515625" style="22" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="10" max="10" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.33203125" style="22" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="1"/>
     <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="1" customWidth="1"/>
-    <col min="17" max="17" width="22.7109375" style="1" customWidth="1"/>
-    <col min="18" max="19" width="9.140625" style="1"/>
+    <col min="17" max="17" width="22.6640625" style="1" customWidth="1"/>
+    <col min="18" max="19" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-    </row>
-    <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
-      <c r="H4" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="33"/>
-      <c r="N4" s="31" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+    </row>
+    <row r="3" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40"/>
+      <c r="H4" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="40"/>
+      <c r="N4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="33"/>
-    </row>
-    <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="40"/>
+    </row>
+    <row r="5" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1440,19 +1474,19 @@
         <v>23</v>
       </c>
       <c r="P5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q5" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="Q5" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="R5" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S5" s="27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C6" s="4">
         <v>1</v>
       </c>
@@ -1460,7 +1494,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" s="4">
         <v>123456</v>
@@ -1469,13 +1503,13 @@
         <v>1</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J6" s="4">
         <v>1</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L6" s="5">
         <v>123456</v>
@@ -1499,15 +1533,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C7" s="20">
         <v>2</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" s="4">
         <v>123456</v>
@@ -1516,13 +1550,13 @@
         <v>2</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J7" s="20">
         <v>1</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L7" s="5">
         <v>123456</v>
@@ -1546,15 +1580,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C8" s="20">
         <v>3</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" s="4">
         <v>123456</v>
@@ -1563,13 +1597,13 @@
         <v>3</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J8" s="20">
         <v>2</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L8" s="5">
         <v>123456</v>
@@ -1581,7 +1615,7 @@
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
@@ -1590,13 +1624,13 @@
         <v>4</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J9" s="20">
         <v>2</v>
       </c>
       <c r="K9" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L9" s="5">
         <v>123456</v>
@@ -1608,7 +1642,7 @@
       <c r="R9" s="20"/>
       <c r="S9" s="20"/>
     </row>
-    <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -1627,18 +1661,18 @@
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
     </row>
-    <row r="17" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I18" s="36" t="s">
+    <row r="17" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="L18" s="36"/>
+      <c r="L18" s="43"/>
       <c r="M18" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N18" s="23" t="s">
         <v>2</v>
@@ -1647,22 +1681,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="31" t="s">
+    <row r="19" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="33"/>
+      <c r="D19" s="40"/>
       <c r="J19" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L19" s="1">
         <v>1</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
@@ -1676,10 +1710,10 @@
         <v>2</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C21" s="10">
         <v>1</v>
       </c>
@@ -1687,16 +1721,16 @@
         <v>16</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L21" s="1">
         <v>3</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C22" s="12">
         <v>2</v>
       </c>
@@ -1707,10 +1741,10 @@
         <v>4</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C23" s="14">
         <v>3</v>
       </c>
@@ -1721,131 +1755,130 @@
         <v>5</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.3">
       <c r="L24" s="1">
         <v>6</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.3">
       <c r="L25" s="1">
         <v>7</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.3">
       <c r="L26" s="1">
         <v>8</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.3">
       <c r="L27" s="1">
         <v>9</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.3">
       <c r="L28" s="1">
         <v>10</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M29" s="19"/>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M30" s="19"/>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="M29" s="36"/>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="M30" s="36"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.3">
       <c r="J31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M31" s="19"/>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M32" s="19"/>
-    </row>
-    <row r="33" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M33" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="N33" s="35"/>
-      <c r="O33" s="35"/>
-      <c r="P33" s="35"/>
-      <c r="Q33" s="35"/>
-      <c r="R33" s="35"/>
-      <c r="S33" s="35"/>
-    </row>
-    <row r="34" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J34" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="M31" s="36"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="M32" s="36"/>
+    </row>
+    <row r="33" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="M33" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="N33" s="42"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="42"/>
+      <c r="Q33" s="42"/>
+      <c r="R33" s="42"/>
+      <c r="S33" s="42"/>
+    </row>
+    <row r="34" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="J34" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="K34" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="K34" s="22" t="s">
+      <c r="M34" s="36"/>
+    </row>
+    <row r="35" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="K35" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="M34" s="19"/>
-    </row>
-    <row r="35" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="K35" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="M35" s="19"/>
+      <c r="M35" s="36"/>
       <c r="N35" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O35" s="6">
         <v>44509</v>
       </c>
       <c r="P35" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q35" s="30">
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M36" s="19"/>
-    </row>
-    <row r="37" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M37" s="19"/>
-    </row>
-    <row r="38" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M38" s="19"/>
-    </row>
-    <row r="39" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M39" s="19"/>
+    <row r="36" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="M36" s="36"/>
+    </row>
+    <row r="37" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="M37" s="36"/>
+    </row>
+    <row r="38" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="M38" s="36"/>
+    </row>
+    <row r="39" spans="10:19" x14ac:dyDescent="0.3">
+      <c r="M39" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C19:D19"/>
     <mergeCell ref="M33:S33"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="H4:L4"/>
     <mergeCell ref="N4:S4"/>
-    <mergeCell ref="C19:D19"/>
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="K18:L18"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K6" r:id="rId1" xr:uid="{8A8A762A-B7E7-471E-AA59-31CF2E500441}"/>
-    <hyperlink ref="K7" r:id="rId2" xr:uid="{83738695-7ABB-4B89-B0EA-022F19AE12A1}"/>
-    <hyperlink ref="K8" r:id="rId3" xr:uid="{8F57AA61-C263-4330-804C-7EC8070D3E98}"/>
-    <hyperlink ref="K9" r:id="rId4" xr:uid="{3B05CF7C-D890-44CD-A32E-D265B4DC0B91}"/>
+    <hyperlink ref="K6" r:id="rId1" xr:uid="{8CD205EB-F179-498B-98FC-A2E47B7AB2DA}"/>
+    <hyperlink ref="K7" r:id="rId2" xr:uid="{B91D99AA-AB1C-4BEC-93BD-5EC77572883E}"/>
+    <hyperlink ref="K8" r:id="rId3" xr:uid="{66FE94C6-D258-4725-B6FC-704EF1336BCA}"/>
+    <hyperlink ref="K9" r:id="rId4" xr:uid="{6BB8E1F4-CE2F-49E0-8A93-D50A3C822DC9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -1853,41 +1886,566 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21980860-3ED3-4236-B456-9214120E1B2A}">
+  <dimension ref="B2:R38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="32.33203125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="1"/>
+    <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" style="1" customWidth="1"/>
+    <col min="16" max="16" width="22.6640625" style="1" customWidth="1"/>
+    <col min="17" max="18" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+    </row>
+    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="40"/>
+      <c r="F4" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="40"/>
+      <c r="M4" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="40"/>
+    </row>
+    <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R5" s="27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="K6" s="5">
+        <v>123456</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
+      <c r="N6" s="4">
+        <v>1</v>
+      </c>
+      <c r="O6" s="6">
+        <v>44509</v>
+      </c>
+      <c r="P6" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>6</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C7" s="20">
+        <v>2</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="20">
+        <v>2</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="20">
+        <v>2</v>
+      </c>
+      <c r="I7" s="20">
+        <v>2</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="5">
+        <v>123456</v>
+      </c>
+      <c r="M7" s="20">
+        <v>2</v>
+      </c>
+      <c r="N7" s="20">
+        <v>1</v>
+      </c>
+      <c r="O7" s="21">
+        <v>44501</v>
+      </c>
+      <c r="P7" s="20">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="20">
+        <v>20</v>
+      </c>
+      <c r="R7" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C8" s="20">
+        <v>3</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="20">
+        <v>3</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" s="20">
+        <v>2</v>
+      </c>
+      <c r="I8" s="20">
+        <v>1</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="K8" s="5">
+        <v>123456</v>
+      </c>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="F9" s="20">
+        <v>4</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="20">
+        <v>2</v>
+      </c>
+      <c r="I9" s="20">
+        <v>2</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="5">
+        <v>123456</v>
+      </c>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+    </row>
+    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="F10" s="7">
+        <v>5</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="8"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+    </row>
+    <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="40"/>
+    </row>
+    <row r="14" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C15" s="10">
+        <v>1</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="14">
+        <v>2</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G17" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" s="43"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="K17" s="43"/>
+      <c r="L17" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="M17" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="40"/>
+      <c r="H18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="1">
+        <v>2</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C20" s="10">
+        <v>1</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K20" s="1">
+        <v>3</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C21" s="12">
+        <v>2</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="1">
+        <v>4</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="14">
+        <v>3</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K22" s="1">
+        <v>5</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="K23" s="1">
+        <v>6</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="K24" s="1">
+        <v>7</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="K25" s="1">
+        <v>8</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="K26" s="1">
+        <v>9</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="K27" s="1">
+        <v>10</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="L28" s="19"/>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="L29" s="19"/>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="H30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L30" s="19"/>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="L31" s="19"/>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="L32" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="M32" s="42"/>
+      <c r="N32" s="42"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="42"/>
+      <c r="Q32" s="42"/>
+      <c r="R32" s="42"/>
+    </row>
+    <row r="33" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H33" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" s="37"/>
+      <c r="J33" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="L33" s="19"/>
+    </row>
+    <row r="34" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="J34" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="L34" s="19"/>
+      <c r="M34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N34" s="6">
+        <v>44509</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="P34" s="30">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="L35" s="19"/>
+    </row>
+    <row r="36" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="L36" s="19"/>
+    </row>
+    <row r="37" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="L37" s="19"/>
+    </row>
+    <row r="38" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="L38" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="L32:R32"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="M4:R4"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="C13:D13"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J6" r:id="rId1" xr:uid="{8A8A762A-B7E7-471E-AA59-31CF2E500441}"/>
+    <hyperlink ref="J7" r:id="rId2" xr:uid="{83738695-7ABB-4B89-B0EA-022F19AE12A1}"/>
+    <hyperlink ref="J8" r:id="rId3" xr:uid="{8F57AA61-C263-4330-804C-7EC8070D3E98}"/>
+    <hyperlink ref="J9" r:id="rId4" xr:uid="{3B05CF7C-D890-44CD-A32E-D265B4DC0B91}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101C0A5E-53D3-4EE9-8425-C86F54FEF2B4}">
   <dimension ref="B1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="55.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="55.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1897,11 +2455,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="32" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="16" t="s">
@@ -1911,11 +2469,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="32" t="s">
         <v>31</v>
       </c>
       <c r="D5" s="16" t="s">
@@ -1925,170 +2483,183 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="31" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="32" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="34"/>
+      <c r="G9" s="35"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="40"/>
-      <c r="G9" s="41"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="32" t="s">
         <v>26</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="32" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="32" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>42</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="38" t="s">
-        <v>26</v>
+      <c r="C14" s="32" t="s">
+        <v>29</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="32" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="35"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7"/>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="33" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating the style of v2 database
</commit_message>
<xml_diff>
--- a/BD-Onboard.xlsx
+++ b/BD-Onboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JR\Documents\Edu\Univ\DWM-IPCA\02_S1-DCS\TP\WIP\OnboardDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D683FF-7960-4FF6-9546-E101B5ABC364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D125D104-4A7C-460A-8070-610DDB47C955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21980860-3ED3-4236-B456-9214120E1B2A}">
   <dimension ref="B2:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1901,14 +1901,14 @@
     <col min="5" max="6" width="9.109375" style="1"/>
     <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32.33203125" style="22" customWidth="1"/>
     <col min="11" max="11" width="9.109375" style="1"/>
     <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18" style="1" customWidth="1"/>
-    <col min="16" max="16" width="22.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="9.109375" style="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Updating the onboard documentation page
</commit_message>
<xml_diff>
--- a/BD-Onboard.xlsx
+++ b/BD-Onboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JR\Documents\Edu\Univ\DWM-IPCA\02_S1-DCS\TP\WIP\OnboardDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC914070-789E-4526-95B8-0591CBCFDD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B6EE08-5E37-438A-A909-7004829E00FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="1884" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RESTFull URL" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="124">
   <si>
     <t>Base de Dados</t>
   </si>
@@ -130,9 +130,6 @@
     <t>getUser</t>
   </si>
   <si>
-    <t>updateUser</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
   </si>
   <si>
     <t>Business Operation</t>
-  </si>
-  <si>
-    <t>DeleteUser</t>
   </si>
   <si>
     <t>company name</t>
@@ -351,18 +345,9 @@
     <t>/v1/Transactions/; { user_id }</t>
   </si>
   <si>
-    <t>getUserTransactions</t>
-  </si>
-  <si>
     <t>Transaction</t>
   </si>
   <si>
-    <t>createTransaction</t>
-  </si>
-  <si>
-    <t>updateTransaction</t>
-  </si>
-  <si>
     <t>deleteTransaction</t>
   </si>
   <si>
@@ -412,6 +397,36 @@
   </si>
   <si>
     <t>Food</t>
+  </si>
+  <si>
+    <t>getCompanies</t>
+  </si>
+  <si>
+    <t>/Auth/Signup/; { company_id }</t>
+  </si>
+  <si>
+    <t>getUsers</t>
+  </si>
+  <si>
+    <t>editUser</t>
+  </si>
+  <si>
+    <t>deleteUser</t>
+  </si>
+  <si>
+    <t>postTransaction</t>
+  </si>
+  <si>
+    <t>editTransaction</t>
+  </si>
+  <si>
+    <t>getCategories</t>
+  </si>
+  <si>
+    <t>/v1/Transactions/categories/; &lt;CategoriesData&gt;</t>
+  </si>
+  <si>
+    <t>getTransactions</t>
   </si>
 </sst>
 </file>
@@ -965,9 +980,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1084,23 +1096,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1453,10 +1468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101C0A5E-53D3-4EE9-8425-C86F54FEF2B4}">
-  <dimension ref="B1:G12"/>
+  <dimension ref="B1:G15"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E15" sqref="B2:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,27 +1485,27 @@
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="60" t="s">
         <v>36</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>29</v>
@@ -1498,13 +1513,13 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>30</v>
@@ -1512,118 +1527,160 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>28</v>
+        <v>92</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>31</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>33</v>
+        <v>94</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>28</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="34"/>
+        <v>117</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>27</v>
+        <v>94</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>98</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>26</v>
+        <v>95</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>28</v>
+        <v>100</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>26</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>33</v>
+        <v>98</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>28</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="34"/>
-    </row>
-    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" s="32" t="s">
+      <c r="D13" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>110</v>
+      <c r="D14" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1636,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21980860-3ED3-4236-B456-9214120E1B2A}">
   <dimension ref="A2:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,7 +1711,7 @@
     <col min="12" max="12" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="22" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="21" customWidth="1"/>
     <col min="16" max="16" width="9.140625" style="1"/>
     <col min="17" max="17" width="3" style="1" customWidth="1"/>
     <col min="18" max="18" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1666,120 +1723,120 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="66"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="61" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="63" t="s">
+      <c r="B4" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="63"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="66"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="66"/>
+      <c r="K4" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="65"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="63" t="s">
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="66"/>
+      <c r="R4" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="I4" s="65"/>
-      <c r="K4" s="63" t="s">
-        <v>86</v>
-      </c>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="65"/>
-      <c r="R4" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="S4" s="64"/>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="65"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="65"/>
+      <c r="U4" s="65"/>
+      <c r="V4" s="65"/>
+      <c r="W4" s="66"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" s="51"/>
+        <v>108</v>
+      </c>
+      <c r="D5" s="50"/>
       <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G5" s="51"/>
+        <v>109</v>
+      </c>
+      <c r="G5" s="50"/>
       <c r="H5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="N5" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="N5" s="22" t="s">
         <v>2</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="S5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="T5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="V5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="W5" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="W5" s="26" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1790,19 +1847,19 @@
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="38"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="10">
         <v>1</v>
       </c>
-      <c r="F6" s="59" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="38"/>
+      <c r="F6" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="37"/>
       <c r="H6" s="10">
         <v>1</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K6" s="4">
         <v>1</v>
@@ -1811,10 +1868,10 @@
         <v>1</v>
       </c>
       <c r="M6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N6" s="25" t="s">
         <v>77</v>
-      </c>
-      <c r="N6" s="26" t="s">
-        <v>79</v>
       </c>
       <c r="O6" s="5">
         <v>123456</v>
@@ -1842,320 +1899,320 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="20">
-        <v>2</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="38"/>
+      <c r="B7" s="19">
+        <v>2</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="37"/>
       <c r="E7" s="14">
         <v>2</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="38"/>
+        <v>31</v>
+      </c>
+      <c r="G7" s="37"/>
       <c r="H7" s="12">
         <v>2</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="K7" s="20">
-        <v>2</v>
-      </c>
-      <c r="L7" s="20">
+        <v>112</v>
+      </c>
+      <c r="K7" s="19">
+        <v>2</v>
+      </c>
+      <c r="L7" s="19">
         <v>1</v>
       </c>
-      <c r="M7" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="N7" s="26" t="s">
-        <v>57</v>
+      <c r="M7" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="25" t="s">
+        <v>55</v>
       </c>
       <c r="O7" s="5">
         <v>123456</v>
       </c>
-      <c r="P7" s="20">
-        <v>2</v>
-      </c>
-      <c r="R7" s="20">
-        <v>2</v>
-      </c>
-      <c r="S7" s="20">
+      <c r="P7" s="19">
+        <v>2</v>
+      </c>
+      <c r="R7" s="19">
+        <v>2</v>
+      </c>
+      <c r="S7" s="19">
         <v>1</v>
       </c>
-      <c r="T7" s="21">
+      <c r="T7" s="20">
         <v>44501</v>
       </c>
-      <c r="U7" s="20">
-        <v>2</v>
-      </c>
-      <c r="V7" s="20">
+      <c r="U7" s="19">
+        <v>2</v>
+      </c>
+      <c r="V7" s="19">
         <v>100</v>
       </c>
-      <c r="W7" s="20" t="s">
+      <c r="W7" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="20">
+      <c r="B8" s="19">
         <v>3</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="C8" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="14">
         <v>3</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="K8" s="20">
+        <v>113</v>
+      </c>
+      <c r="K8" s="19">
         <v>3</v>
       </c>
-      <c r="L8" s="20">
-        <v>2</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="N8" s="24" t="s">
-        <v>60</v>
+      <c r="L8" s="19">
+        <v>2</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="23" t="s">
+        <v>58</v>
       </c>
       <c r="O8" s="5">
         <v>123456</v>
       </c>
-      <c r="P8" s="20">
+      <c r="P8" s="19">
         <v>1</v>
       </c>
-      <c r="R8" s="20">
+      <c r="R8" s="19">
         <v>3</v>
       </c>
-      <c r="S8" s="20">
-        <v>2</v>
-      </c>
-      <c r="T8" s="21">
+      <c r="S8" s="19">
+        <v>2</v>
+      </c>
+      <c r="T8" s="20">
         <v>44532</v>
       </c>
-      <c r="U8" s="20">
+      <c r="U8" s="19">
         <v>1</v>
       </c>
-      <c r="V8" s="20">
+      <c r="V8" s="19">
         <v>200</v>
       </c>
-      <c r="W8" s="20" t="s">
+      <c r="W8" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="48">
+      <c r="B9" s="47">
         <v>4</v>
       </c>
-      <c r="C9" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="K9" s="20">
+      <c r="C9" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="K9" s="19">
         <v>4</v>
       </c>
-      <c r="L9" s="20">
-        <v>2</v>
-      </c>
-      <c r="M9" s="20" t="s">
+      <c r="L9" s="19">
+        <v>2</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="N9" s="23" t="s">
         <v>59</v>
-      </c>
-      <c r="N9" s="24" t="s">
-        <v>61</v>
       </c>
       <c r="O9" s="5">
         <v>123456</v>
       </c>
-      <c r="P9" s="20">
-        <v>2</v>
-      </c>
-      <c r="R9" s="20">
+      <c r="P9" s="19">
+        <v>2</v>
+      </c>
+      <c r="R9" s="19">
         <v>4</v>
       </c>
-      <c r="S9" s="20">
-        <v>2</v>
-      </c>
-      <c r="T9" s="21">
+      <c r="S9" s="19">
+        <v>2</v>
+      </c>
+      <c r="T9" s="20">
         <v>44532</v>
       </c>
-      <c r="U9" s="20">
+      <c r="U9" s="19">
         <v>3</v>
       </c>
-      <c r="V9" s="20">
+      <c r="V9" s="19">
         <v>10</v>
       </c>
-      <c r="W9" s="20" t="s">
+      <c r="W9" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
       <c r="K10" s="7">
         <v>5</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
-      <c r="O10" s="25"/>
+      <c r="O10" s="24"/>
       <c r="P10" s="8"/>
       <c r="R10" s="7">
         <v>5</v>
       </c>
       <c r="S10" s="7"/>
       <c r="T10" s="9"/>
-      <c r="U10" s="37"/>
+      <c r="U10" s="36"/>
       <c r="V10" s="7"/>
       <c r="W10" s="7"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="40"/>
-      <c r="U11" s="41"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="39"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="37"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="40"/>
-      <c r="U12" s="41"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="38"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="39"/>
+      <c r="U12" s="40"/>
+      <c r="V12" s="37"/>
+      <c r="W12" s="37"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="60"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="59"/>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
     </row>
     <row r="37" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q37" s="19"/>
+      <c r="Q37" s="18"/>
     </row>
     <row r="38" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q38" s="19"/>
+      <c r="Q38" s="18"/>
     </row>
     <row r="39" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q39" s="19"/>
+      <c r="Q39" s="18"/>
     </row>
     <row r="40" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q40" s="19"/>
+      <c r="Q40" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2191,18 +2248,18 @@
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="71" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="72"/>
-      <c r="D2" s="36"/>
+      <c r="D2" s="35"/>
       <c r="F2" s="71" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G2" s="73"/>
       <c r="H2" s="73"/>
       <c r="I2" s="72"/>
       <c r="K2" s="71" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L2" s="73"/>
       <c r="M2" s="73"/>
@@ -2212,25 +2269,25 @@
       <c r="Q2" s="72"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="42"/>
-      <c r="C3" s="43" t="s">
-        <v>39</v>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42" t="s">
+        <v>37</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="F3" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="52" t="s">
+      <c r="F3" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="51" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="74" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L3" s="75"/>
       <c r="M3" s="75"/>
@@ -2240,61 +2297,61 @@
       <c r="Q3" s="76"/>
     </row>
     <row r="4" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="42"/>
-      <c r="C4" s="43" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="42" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="42">
+      <c r="E4" s="21"/>
+      <c r="F4" s="41">
         <v>1</v>
       </c>
-      <c r="G4" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="43"/>
-      <c r="K4" s="53" t="s">
-        <v>112</v>
-      </c>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="55"/>
+      <c r="G4" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="37"/>
+      <c r="I4" s="42"/>
+      <c r="K4" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="54"/>
     </row>
     <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="44"/>
-      <c r="C5" s="45" t="s">
-        <v>40</v>
+      <c r="B5" s="43"/>
+      <c r="C5" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="42">
-        <v>2</v>
-      </c>
-      <c r="G5" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="43"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="41">
+        <v>2</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="37"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="42">
+      <c r="E6" s="21"/>
+      <c r="F6" s="41">
         <v>3</v>
       </c>
-      <c r="G6" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="43"/>
+      <c r="G6" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="37"/>
+      <c r="I6" s="42"/>
       <c r="K6" s="67" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L6" s="68"/>
       <c r="M6" s="68"/>
@@ -2304,25 +2361,25 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="42">
+      <c r="E7" s="21"/>
+      <c r="F7" s="41">
         <v>4</v>
       </c>
-      <c r="G7" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="38"/>
-      <c r="I7" s="43"/>
+      <c r="G7" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="37"/>
+      <c r="I7" s="42"/>
       <c r="K7" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" s="56">
+        <v>39</v>
+      </c>
+      <c r="L7" s="55">
         <v>44509</v>
       </c>
-      <c r="M7" s="57" t="s">
-        <v>72</v>
-      </c>
-      <c r="N7" s="58">
+      <c r="M7" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="N7" s="57">
         <v>200</v>
       </c>
     </row>
@@ -2330,93 +2387,93 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="42">
+      <c r="E8" s="21"/>
+      <c r="F8" s="41">
         <v>5</v>
       </c>
-      <c r="G8" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="38"/>
-      <c r="I8" s="43"/>
+      <c r="G8" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="37"/>
+      <c r="I8" s="42"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="42">
+      <c r="E9" s="21"/>
+      <c r="F9" s="41">
         <v>6</v>
       </c>
-      <c r="G9" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="38"/>
-      <c r="I9" s="43"/>
+      <c r="G9" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="37"/>
+      <c r="I9" s="42"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="42">
+      <c r="E10" s="21"/>
+      <c r="F10" s="41">
         <v>7</v>
       </c>
-      <c r="G10" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="38"/>
-      <c r="I10" s="43"/>
+      <c r="G10" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="37"/>
+      <c r="I10" s="42"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="42">
+      <c r="E11" s="21"/>
+      <c r="F11" s="41">
         <v>8</v>
       </c>
-      <c r="G11" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="38"/>
-      <c r="I11" s="43"/>
+      <c r="G11" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="37"/>
+      <c r="I11" s="42"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="42">
+      <c r="E12" s="21"/>
+      <c r="F12" s="41">
         <v>9</v>
       </c>
-      <c r="G12" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="38"/>
-      <c r="I12" s="43"/>
+      <c r="G12" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="37"/>
+      <c r="I12" s="42"/>
     </row>
     <row r="13" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="44">
+      <c r="E13" s="21"/>
+      <c r="F13" s="43">
         <v>10</v>
       </c>
-      <c r="G13" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="49"/>
-      <c r="I13" s="45"/>
+      <c r="G13" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="48"/>
+      <c r="I13" s="44"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="22"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="38"/>
+      <c r="G14" s="37"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -2428,9 +2485,9 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="22"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="38"/>
+      <c r="G15" s="37"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -2442,9 +2499,9 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="22"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="19"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -2454,11 +2511,11 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="38"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="22"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="19"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -2470,9 +2527,9 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="22"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="19"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2484,7 +2541,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="22"/>
+      <c r="E19" s="21"/>
       <c r="F19" s="1"/>
       <c r="G19" s="70"/>
       <c r="H19" s="70"/>
@@ -2496,9 +2553,9 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="E20" s="22"/>
+      <c r="E20" s="21"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="19"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2510,9 +2567,9 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="22"/>
+      <c r="E21" s="21"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="19"/>
+      <c r="G21" s="18"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
@@ -2562,27 +2619,27 @@
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="65"/>
-      <c r="H4" s="63" t="s">
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="66"/>
+      <c r="H4" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="65"/>
-      <c r="N4" s="63" t="s">
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="66"/>
+      <c r="N4" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="64"/>
-      <c r="S4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="66"/>
     </row>
     <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
@@ -2711,10 +2768,10 @@
     </row>
     <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="65"/>
+      <c r="D12" s="66"/>
     </row>
     <row r="13" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
@@ -2777,7 +2834,7 @@
     <col min="5" max="8" width="8.85546875" style="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.28515625" style="22" customWidth="1"/>
+    <col min="11" max="11" width="32.28515625" style="21" customWidth="1"/>
     <col min="12" max="12" width="8.85546875" style="1"/>
     <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -2796,27 +2853,27 @@
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="65"/>
-      <c r="H4" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="65"/>
-      <c r="N4" s="63" t="s">
+      <c r="C4" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="66"/>
+      <c r="H4" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="66"/>
+      <c r="N4" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="64"/>
-      <c r="S4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="66"/>
     </row>
     <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
@@ -2840,7 +2897,7 @@
       <c r="J5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="22" t="s">
         <v>2</v>
       </c>
       <c r="L5" s="3" t="s">
@@ -2853,15 +2910,15 @@
         <v>23</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="S5" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="S5" s="26" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2873,7 +2930,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F6" s="4">
         <v>123456</v>
@@ -2882,13 +2939,13 @@
         <v>1</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J6" s="4">
         <v>1</v>
       </c>
-      <c r="K6" s="26" t="s">
-        <v>56</v>
+      <c r="K6" s="25" t="s">
+        <v>54</v>
       </c>
       <c r="L6" s="5">
         <v>123456</v>
@@ -2913,113 +2970,113 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C7" s="20">
-        <v>2</v>
-      </c>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="19">
+        <v>2</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="19" t="s">
         <v>51</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>53</v>
       </c>
       <c r="F7" s="4">
         <v>123456</v>
       </c>
-      <c r="H7" s="20">
-        <v>2</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" s="20">
+      <c r="H7" s="19">
+        <v>2</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="19">
         <v>1</v>
       </c>
-      <c r="K7" s="26" t="s">
-        <v>57</v>
+      <c r="K7" s="25" t="s">
+        <v>55</v>
       </c>
       <c r="L7" s="5">
         <v>123456</v>
       </c>
-      <c r="N7" s="20">
-        <v>2</v>
-      </c>
-      <c r="O7" s="20">
+      <c r="N7" s="19">
+        <v>2</v>
+      </c>
+      <c r="O7" s="19">
         <v>1</v>
       </c>
-      <c r="P7" s="21">
+      <c r="P7" s="20">
         <v>44501</v>
       </c>
-      <c r="Q7" s="20">
-        <v>2</v>
-      </c>
-      <c r="R7" s="20">
+      <c r="Q7" s="19">
+        <v>2</v>
+      </c>
+      <c r="R7" s="19">
         <v>20</v>
       </c>
-      <c r="S7" s="20" t="s">
+      <c r="S7" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C8" s="20">
+      <c r="C8" s="19">
         <v>3</v>
       </c>
-      <c r="D8" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>54</v>
+      <c r="D8" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="F8" s="4">
         <v>123456</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="19">
         <v>3</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="19">
+        <v>2</v>
+      </c>
+      <c r="K8" s="23" t="s">
         <v>58</v>
-      </c>
-      <c r="J8" s="20">
-        <v>2</v>
-      </c>
-      <c r="K8" s="24" t="s">
-        <v>60</v>
       </c>
       <c r="L8" s="5">
         <v>123456</v>
       </c>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="4"/>
-      <c r="H9" s="20">
+      <c r="H9" s="19">
         <v>4</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="19">
+        <v>2</v>
+      </c>
+      <c r="K9" s="23" t="s">
         <v>59</v>
-      </c>
-      <c r="J9" s="20">
-        <v>2</v>
-      </c>
-      <c r="K9" s="24" t="s">
-        <v>61</v>
       </c>
       <c r="L9" s="5">
         <v>123456</v>
       </c>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
     </row>
     <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="7"/>
@@ -3031,7 +3088,7 @@
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="25"/>
+      <c r="K10" s="24"/>
       <c r="L10" s="8"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
@@ -3043,17 +3100,17 @@
     <row r="17" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I18" s="78" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J18" s="78"/>
       <c r="K18" s="78" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L18" s="78"/>
-      <c r="M18" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="N18" s="23" t="s">
+      <c r="M18" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="N18" s="22" t="s">
         <v>2</v>
       </c>
       <c r="O18" s="3" t="s">
@@ -3061,18 +3118,18 @@
       </c>
     </row>
     <row r="19" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="63" t="s">
+      <c r="C19" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="65"/>
+      <c r="D19" s="66"/>
       <c r="J19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L19" s="1">
         <v>1</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3089,7 +3146,7 @@
         <v>2</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
@@ -3100,13 +3157,13 @@
         <v>16</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L21" s="1">
         <v>3</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.25">
@@ -3120,7 +3177,7 @@
         <v>4</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3134,7 +3191,7 @@
         <v>5</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
@@ -3142,7 +3199,7 @@
         <v>6</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.25">
@@ -3150,7 +3207,7 @@
         <v>7</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.25">
@@ -3158,7 +3215,7 @@
         <v>8</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.25">
@@ -3166,7 +3223,7 @@
         <v>9</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.25">
@@ -3174,27 +3231,27 @@
         <v>10</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M29" s="35"/>
+      <c r="M29" s="34"/>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M30" s="35"/>
+      <c r="M30" s="34"/>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
       <c r="J31" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="M31" s="35"/>
+        <v>65</v>
+      </c>
+      <c r="M31" s="34"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M32" s="35"/>
+      <c r="M32" s="34"/>
     </row>
     <row r="33" spans="10:19" x14ac:dyDescent="0.25">
       <c r="M33" s="70" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N33" s="70"/>
       <c r="O33" s="70"/>
@@ -3204,43 +3261,43 @@
       <c r="S33" s="70"/>
     </row>
     <row r="34" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="J34" s="36" t="s">
+      <c r="J34" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="K34" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="M34" s="34"/>
+    </row>
+    <row r="35" spans="10:19" x14ac:dyDescent="0.25">
+      <c r="K35" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="K34" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="M34" s="35"/>
-    </row>
-    <row r="35" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="K35" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="M35" s="35"/>
+      <c r="M35" s="34"/>
       <c r="N35" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O35" s="6">
         <v>44509</v>
       </c>
       <c r="P35" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q35" s="29">
+        <v>70</v>
+      </c>
+      <c r="Q35" s="28">
         <v>200</v>
       </c>
     </row>
     <row r="36" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M36" s="35"/>
+      <c r="M36" s="34"/>
     </row>
     <row r="37" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M37" s="35"/>
+      <c r="M37" s="34"/>
     </row>
     <row r="38" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M38" s="35"/>
+      <c r="M38" s="34"/>
     </row>
     <row r="39" spans="10:19" x14ac:dyDescent="0.25">
-      <c r="M39" s="35"/>
+      <c r="M39" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>